<commit_message>
updated chap 5 summary
</commit_message>
<xml_diff>
--- a/figures/5_Ascent/BarChart1.xlsx
+++ b/figures/5_Ascent/BarChart1.xlsx
@@ -16,28 +16,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>Dynamic Pressure</t>
+    <t>Third Stage Specific Impulse</t>
   </si>
   <si>
-    <t>Cd</t>
+    <t>SPARTAN Specific Impulse</t>
   </si>
   <si>
-    <t>Isp</t>
+    <t>SPARTAN Drag</t>
   </si>
   <si>
-    <t>mFuel2</t>
+    <t>SPARTAN Structural Mass</t>
   </si>
   <si>
-    <t>m3</t>
+    <t>Third Stage Mass</t>
   </si>
   <si>
-    <t>m2</t>
+    <t>SPARTAN Fuel Mass</t>
   </si>
   <si>
-    <t>Cd3</t>
+    <t>Maximum Dynamic Pressure</t>
   </si>
   <si>
-    <t>Isp3</t>
+    <t>Third Stage Drag</t>
   </si>
 </sst>
 </file>
@@ -113,11 +113,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -127,8 +127,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-AU"/>
-              <a:t>Payload Per % Variation</a:t>
+              <a:t>Payload Variation</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" baseline="0"/>
+              <a:t> (kg) per % Parameter Variation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -146,11 +151,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -166,7 +171,7 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="col"/>
+        <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -174,42 +179,172 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent1">
+                <a:alpha val="85000"/>
+              </a:schemeClr>
             </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.2467138199161134E-3"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5437593084481274E-2"/>
+                  <c:y val="-8.4875562720133283E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$1:$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>Cd3</c:v>
+                  <c:v>Third Stage Drag</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Dynamic Pressure</c:v>
+                  <c:v>Maximum Dynamic Pressure</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>mFuel2</c:v>
+                  <c:v>SPARTAN Fuel Mass</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>m3</c:v>
+                  <c:v>Third Stage Mass</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>m2</c:v>
+                  <c:v>SPARTAN Structural Mass</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Cd</c:v>
+                  <c:v>SPARTAN Drag</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Isp</c:v>
+                  <c:v>SPARTAN Specific Impulse</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Isp3</c:v>
+                  <c:v>Third Stage Specific Impulse</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -249,36 +384,36 @@
           </c:val>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="492188184"/>
-        <c:axId val="492188968"/>
+        <c:gapWidth val="65"/>
+        <c:axId val="219788224"/>
+        <c:axId val="220158968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="492188184"/>
+        <c:axId val="219788224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -290,11 +425,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -305,29 +440,42 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492188968"/>
+        <c:crossAx val="220158968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
+        <c:lblOffset val="0"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="492188968"/>
+        <c:axId val="220158968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="-2"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="95000"/>
+                      <a:lumOff val="5000"/>
+                      <a:alpha val="42000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="36000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -351,9 +499,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -364,7 +512,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492188184"/>
+        <c:crossAx val="219788224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -382,13 +530,13 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:round/>
@@ -454,171 +602,207 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="218">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="75000"/>
         <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="dk1">
             <a:lumMod val="25000"/>
             <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -634,21 +818,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -663,13 +845,13 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -682,17 +864,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -701,12 +883,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -720,30 +902,36 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -753,17 +941,28 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -772,12 +971,88 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="75000"/>
             <a:lumOff val="25000"/>
           </a:schemeClr>
@@ -785,64 +1060,6 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -850,14 +1067,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -869,12 +1086,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -883,14 +1100,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -899,9 +1115,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -919,9 +1135,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -932,11 +1148,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -944,14 +1165,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -961,15 +1176,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:colOff>452576</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>33135</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>453258</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>109335</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1280,36 +1495,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>